<commit_message>
Pesquisar livros em ambos os sites
</commit_message>
<xml_diff>
--- a/Dados e-mails teste.xlsx
+++ b/Dados e-mails teste.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanda\Documents\UiPath\compassEvaBuscaDeLivros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF02452F-C8D8-451B-8028-A8C16355A7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262CA3F6-4CF2-4218-A995-770BAF529722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3CCD623D-CC71-44F9-9CC4-137904687159}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3CCD623D-CC71-44F9-9CC4-137904687159}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
+    <sheet name="Dados ok" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Dados ok'!$A$1:$I$10</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="48">
   <si>
     <t>ID E-mail</t>
   </si>
@@ -159,6 +163,27 @@
   </si>
   <si>
     <t>133 páginas</t>
+  </si>
+  <si>
+    <t>John Fowles</t>
+  </si>
+  <si>
+    <t>George Orwell</t>
+  </si>
+  <si>
+    <t>328 páginas</t>
+  </si>
+  <si>
+    <t>The Child in the Photo</t>
+  </si>
+  <si>
+    <t>280 páginas</t>
+  </si>
+  <si>
+    <t>Completa</t>
+  </si>
+  <si>
+    <t>Incompleta</t>
   </si>
 </sst>
 </file>
@@ -209,13 +234,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,10 +558,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E35059-5ABF-4A09-8AAF-61389575A5BC}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>15902</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>16987</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>22316</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>23364</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>26983</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1984</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>26985</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>32568</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>33698</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>42558</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>56980</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>75682</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>85423</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>99685</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2556A93-4FB6-47FA-B97F-BBCA06C6B14B}">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +878,7 @@
     <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -591,6 +926,9 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -608,6 +946,9 @@
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -625,6 +966,9 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -642,6 +986,9 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -659,6 +1006,9 @@
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -676,6 +1026,9 @@
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -693,56 +1046,48 @@
       <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>75682</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>85423</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>85423</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>99685</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>99685</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pesquisa livros na Amazon
</commit_message>
<xml_diff>
--- a/Dados e-mails teste.xlsx
+++ b/Dados e-mails teste.xlsx
@@ -5,20 +5,22 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanda\Documents\UiPath\compassEvaBuscaDeLivros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\uiPath\compassEvaBuscaDeLivros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2225D83-1CE0-4E8E-B591-46F599EE11EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E0E18E-C322-4E63-8A18-7D3331BABF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{3CCD623D-CC71-44F9-9CC4-137904687159}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{3CCD623D-CC71-44F9-9CC4-137904687159}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
     <sheet name="Dados ok" sheetId="2" r:id="rId2"/>
     <sheet name="Dados Extraidos" sheetId="3" r:id="rId3"/>
-    <sheet name="Planilha2" sheetId="4" r:id="rId4"/>
+    <sheet name="Dados Extraidos USA" sheetId="6" r:id="rId4"/>
+    <sheet name="Planilha2" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Dados Extraidos'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Dados ok'!$A$1:$I$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="80">
   <si>
     <t>ID E-mail</t>
   </si>
@@ -186,12 +188,112 @@
   </si>
   <si>
     <t>Incompleta</t>
+  </si>
+  <si>
+    <t>nomeLivro</t>
+  </si>
+  <si>
+    <t>precoUK</t>
+  </si>
+  <si>
+    <t>freteUK</t>
+  </si>
+  <si>
+    <t>tipoDeCapa</t>
+  </si>
+  <si>
+    <t>The Madness of Crowds: Chief Inspector Gamache Novel Book 17</t>
+  </si>
+  <si>
+    <t>£8.00</t>
+  </si>
+  <si>
+    <t>£24.08 delivery</t>
+  </si>
+  <si>
+    <t>The Seven Husbands of Evelyn Hugo: A Novel</t>
+  </si>
+  <si>
+    <t>£24.61</t>
+  </si>
+  <si>
+    <t>£23.71 delivery</t>
+  </si>
+  <si>
+    <t>Wilder Girls</t>
+  </si>
+  <si>
+    <t>The Paper Palace: The No.1 New York Times Bestseller and Reese Witherspoon Bookclub Pick</t>
+  </si>
+  <si>
+    <t>The Midnight Library: Matt Haig</t>
+  </si>
+  <si>
+    <t>£16.20</t>
+  </si>
+  <si>
+    <t>£23.37 delivery</t>
+  </si>
+  <si>
+    <t>You Have a Match: A Novel</t>
+  </si>
+  <si>
+    <t>The Moonlight Child</t>
+  </si>
+  <si>
+    <t>£13.99</t>
+  </si>
+  <si>
+    <t>£23.43 delivery</t>
+  </si>
+  <si>
+    <t>Get A Life, Chloe Brown: TikTok made me buy it! The perfect feel good romance: discovered on TikTok! The perfect feel good romance</t>
+  </si>
+  <si>
+    <t>£6.84</t>
+  </si>
+  <si>
+    <t>£22.68 delivery</t>
+  </si>
+  <si>
+    <t>The Vanishing Half: Shortlisted for the Women's Prize 2021</t>
+  </si>
+  <si>
+    <t>£12.75</t>
+  </si>
+  <si>
+    <t>£23.72 delivery</t>
+  </si>
+  <si>
+    <t>precoLivro</t>
+  </si>
+  <si>
+    <t>precoFrete</t>
+  </si>
+  <si>
+    <t>The Madness of Crowds: A Novel (Chief Inspector Gamache Novel, 17)</t>
+  </si>
+  <si>
+    <t>The Paper Palace (Reese's Book Club): A Novel</t>
+  </si>
+  <si>
+    <t>The Midnight Library: A Novel</t>
+  </si>
+  <si>
+    <t>Get a Life, Chloe Brown: A Novel (The Brown Sisters, 1)</t>
+  </si>
+  <si>
+    <t>The Vanishing Half: A Novel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="165" formatCode="[$£]#,#00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -236,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -249,6 +351,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,20 +671,21 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -609,7 +714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>15902</v>
       </c>
@@ -629,7 +734,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>16987</v>
       </c>
@@ -649,7 +754,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>22316</v>
       </c>
@@ -669,7 +774,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>23364</v>
       </c>
@@ -687,7 +792,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>26983</v>
       </c>
@@ -705,7 +810,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>26985</v>
       </c>
@@ -725,7 +830,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>32568</v>
       </c>
@@ -743,7 +848,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>33698</v>
       </c>
@@ -763,7 +868,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>42558</v>
       </c>
@@ -783,7 +888,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>56980</v>
       </c>
@@ -803,7 +908,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>75682</v>
       </c>
@@ -823,7 +928,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>85423</v>
       </c>
@@ -843,7 +948,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>99685</v>
       </c>
@@ -875,20 +980,21 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -917,7 +1023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>15902</v>
       </c>
@@ -937,7 +1043,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>16987</v>
       </c>
@@ -957,7 +1063,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>22316</v>
       </c>
@@ -977,7 +1083,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>26985</v>
       </c>
@@ -997,7 +1103,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>33698</v>
       </c>
@@ -1017,7 +1123,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>42558</v>
       </c>
@@ -1037,7 +1143,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>56980</v>
       </c>
@@ -1057,7 +1163,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>85423</v>
       </c>
@@ -1077,7 +1183,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>99685</v>
       </c>
@@ -1106,30 +1212,517 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E053CBF7-5DC5-468C-9B1C-DE6D442B34EC}">
   <sheetPr codeName="Planilha3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A2:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A264" workbookViewId="0">
-      <selection activeCell="A264" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="119.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F138A38-496F-4D03-8A8C-6F443916E222}">
+  <dimension ref="A2:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="62.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="6">
+        <v>15.35</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6">
+        <v>21.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="6">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6">
+        <v>20.79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="6">
+        <v>18.8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6">
+        <v>18.63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6">
+        <v>10.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6">
+        <v>10.32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="6">
+        <v>12.57</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6">
+        <v>19.61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="6">
+        <v>13.29</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="6">
+        <v>20.260000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="6">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="6">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="6">
+        <v>14.24</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="6">
+        <v>20.260000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A403FD22-34E3-4133-97C5-1708056DDF9D}">
   <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>

</xml_diff>

<commit_message>
Ajuste Pesquisa Livros Amazon
</commit_message>
<xml_diff>
--- a/Dados e-mails teste.xlsx
+++ b/Dados e-mails teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\uiPath\compassEvaBuscaDeLivros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E0E18E-C322-4E63-8A18-7D3331BABF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D66BAB-8CF9-4B19-800F-5D4AA7ED750D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{3CCD623D-CC71-44F9-9CC4-137904687159}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{3CCD623D-CC71-44F9-9CC4-137904687159}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="116">
   <si>
     <t>ID E-mail</t>
   </si>
@@ -190,6 +190,105 @@
     <t>Incompleta</t>
   </si>
   <si>
+    <t xml:space="preserve"> The Vanishing Half  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brit Bennett</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 133 páginas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hardcover</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Get A Life, Chloe Brown </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talia Hibbert</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 384 páginas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paperback</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verity  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Colleen Hoover</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 331 páginas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Moonlight Child </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Karen McQuestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 326 páginas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> You have a Match </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Emma Lord</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 320 páginas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Midnight Library </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Matt Haig</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 304 páginas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Paper Palace </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Miranda Cowley Heller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 400 páginas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wilder Girls </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rory Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 368 páginas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hardcover </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Seven Husbands of Evelyn Hugo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Taylor Jenkins Reid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 156 páginas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Madness of Crowds</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Louse Penny</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 448 páginas</t>
+  </si>
+  <si>
     <t>nomeLivro</t>
   </si>
   <si>
@@ -202,6 +301,66 @@
     <t>tipoDeCapa</t>
   </si>
   <si>
+    <t>The Vanishing Half: Shortlisted for the Women's Prize 2021</t>
+  </si>
+  <si>
+    <t>£12.75</t>
+  </si>
+  <si>
+    <t>£23.72 delivery</t>
+  </si>
+  <si>
+    <t>Get A Life, Chloe Brown: TikTok made me buy it! The perfect feel good romance: discovered on TikTok! The perfect feel good romance</t>
+  </si>
+  <si>
+    <t>£6.84</t>
+  </si>
+  <si>
+    <t>£22.68 delivery</t>
+  </si>
+  <si>
+    <t>Verity: The thriller that will capture your heart and blow your mind</t>
+  </si>
+  <si>
+    <t>£5.00</t>
+  </si>
+  <si>
+    <t>£22.55 delivery</t>
+  </si>
+  <si>
+    <t>The Moonlight Child</t>
+  </si>
+  <si>
+    <t>£13.99</t>
+  </si>
+  <si>
+    <t>£23.43 delivery</t>
+  </si>
+  <si>
+    <t>You Have a Match: A Novel</t>
+  </si>
+  <si>
+    <t>The Midnight Library: Matt Haig</t>
+  </si>
+  <si>
+    <t>£16.20</t>
+  </si>
+  <si>
+    <t>£23.37 delivery</t>
+  </si>
+  <si>
+    <t>The Paper Palace: The No.1 New York Times Bestseller and Reese Witherspoon Bookclub Pick</t>
+  </si>
+  <si>
+    <t>Wilder Girls</t>
+  </si>
+  <si>
+    <t>Carrie Soto Is Back: From the author of The Seven Husbands of Evelyn Hugo (California dream (crossover) serie, 4)</t>
+  </si>
+  <si>
+    <t>£23.88 delivery</t>
+  </si>
+  <si>
     <t>The Madness of Crowds: Chief Inspector Gamache Novel Book 17</t>
   </si>
   <si>
@@ -211,79 +370,28 @@
     <t>£24.08 delivery</t>
   </si>
   <si>
-    <t>The Seven Husbands of Evelyn Hugo: A Novel</t>
-  </si>
-  <si>
-    <t>£24.61</t>
-  </si>
-  <si>
-    <t>£23.71 delivery</t>
-  </si>
-  <si>
-    <t>Wilder Girls</t>
-  </si>
-  <si>
-    <t>The Paper Palace: The No.1 New York Times Bestseller and Reese Witherspoon Bookclub Pick</t>
-  </si>
-  <si>
-    <t>The Midnight Library: Matt Haig</t>
-  </si>
-  <si>
-    <t>£16.20</t>
-  </si>
-  <si>
-    <t>£23.37 delivery</t>
-  </si>
-  <si>
-    <t>You Have a Match: A Novel</t>
-  </si>
-  <si>
-    <t>The Moonlight Child</t>
-  </si>
-  <si>
-    <t>£13.99</t>
-  </si>
-  <si>
-    <t>£23.43 delivery</t>
-  </si>
-  <si>
-    <t>Get A Life, Chloe Brown: TikTok made me buy it! The perfect feel good romance: discovered on TikTok! The perfect feel good romance</t>
-  </si>
-  <si>
-    <t>£6.84</t>
-  </si>
-  <si>
-    <t>£22.68 delivery</t>
-  </si>
-  <si>
-    <t>The Vanishing Half: Shortlisted for the Women's Prize 2021</t>
-  </si>
-  <si>
-    <t>£12.75</t>
-  </si>
-  <si>
-    <t>£23.72 delivery</t>
-  </si>
-  <si>
     <t>precoLivro</t>
   </si>
   <si>
     <t>precoFrete</t>
   </si>
   <si>
+    <t>The Vanishing Half: A Novel</t>
+  </si>
+  <si>
+    <t>Get a Life, Chloe Brown: A Novel (The Brown Sisters, 1)</t>
+  </si>
+  <si>
+    <t>The Midnight Library: A Novel</t>
+  </si>
+  <si>
+    <t>The Paper Palace (Reese's Book Club): A Novel</t>
+  </si>
+  <si>
+    <t>The Seven Husbands of Evelyn Hugo</t>
+  </si>
+  <si>
     <t>The Madness of Crowds: A Novel (Chief Inspector Gamache Novel, 17)</t>
-  </si>
-  <si>
-    <t>The Paper Palace (Reese's Book Club): A Novel</t>
-  </si>
-  <si>
-    <t>The Midnight Library: A Novel</t>
-  </si>
-  <si>
-    <t>Get a Life, Chloe Brown: A Novel (The Brown Sisters, 1)</t>
-  </si>
-  <si>
-    <t>The Vanishing Half: A Novel</t>
   </si>
 </sst>
 </file>
@@ -977,10 +1085,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2556A93-4FB6-47FA-B97F-BBCA06C6B14B}">
   <sheetPr codeName="Planilha2"/>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,183 +1131,203 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>15902</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>99685</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
       </c>
       <c r="I2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>16987</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>85423</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
       </c>
       <c r="I3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>22316</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>75682</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
       </c>
       <c r="I4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>26985</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>56980</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
       </c>
       <c r="I5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>33698</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>42558</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
       </c>
       <c r="I6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>42558</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>33698</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
       </c>
       <c r="I7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>56980</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>26985</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
       </c>
       <c r="I8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>85423</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>22316</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
       </c>
       <c r="I9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>99685</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>16987</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
       </c>
       <c r="I10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>15902</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1212,41 +1340,40 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E053CBF7-5DC5-468C-9B1C-DE6D442B34EC}">
   <sheetPr codeName="Planilha3"/>
-  <dimension ref="A2:F19"/>
+  <dimension ref="A2:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="119.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>12</v>
@@ -1254,189 +1381,217 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>82</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>92</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>82</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>95</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>82</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1447,263 +1602,281 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F138A38-496F-4D03-8A8C-6F443916E222}">
-  <dimension ref="A2:D19"/>
+  <dimension ref="A2:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="6"/>
+    <col min="1" max="1" width="59.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="B3" s="6">
-        <v>15.35</v>
+        <v>14.24</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="6">
-        <v>21.23</v>
+        <v>20.260000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="B5" s="6">
-        <v>19.149999999999999</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D5" s="6">
-        <v>20.79</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B7" s="6">
-        <v>18.8</v>
+        <v>10.49</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D7" s="6">
-        <v>18.63</v>
+        <v>18.96</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="6">
-        <v>10.88</v>
+        <v>94</v>
+      </c>
+      <c r="B9" s="6">
+        <v>13.29</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="6">
+        <v>20.260000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="6">
-        <v>10.32</v>
+        <v>97</v>
+      </c>
+      <c r="B11" s="6">
+        <v>12.57</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="6">
+        <v>19.61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="6">
-        <v>12.57</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6">
-        <v>19.61</v>
+        <v>112</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>10.32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="6">
-        <v>13.29</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="6">
-        <v>20.260000000000002</v>
+        <v>113</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6">
+        <v>10.88</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B17" s="6">
-        <v>9.9499999999999993</v>
+        <v>18.8</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D17" s="6">
-        <v>18.75</v>
+        <v>18.63</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="6">
-        <v>14.24</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="6">
-        <v>20.260000000000002</v>
+        <v>114</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="6">
+        <v>15.35</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="6">
+        <v>21.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adição de mais try catch
</commit_message>
<xml_diff>
--- a/Dados e-mails teste.xlsx
+++ b/Dados e-mails teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\uiPath\compassEvaBuscaDeLivros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F21FFB-3A1F-40A8-9251-8C47F98563C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8603714-E4C2-4C54-B602-785EDC50475F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3CCD623D-CC71-44F9-9CC4-137904687159}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3CCD623D-CC71-44F9-9CC4-137904687159}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="118">
   <si>
     <t>ID E-mail</t>
   </si>
@@ -311,7 +311,7 @@
     <t>Get A Life, Chloe Brown: TikTok made me buy it! The perfect feel good romance: discovered on TikTok! The perfect feel good romance</t>
   </si>
   <si>
-    <t>£7.14</t>
+    <t>£6.78</t>
   </si>
   <si>
     <t>£22.68 delivery</t>
@@ -338,12 +338,6 @@
     <t>You Have a Match: A Novel</t>
   </si>
   <si>
-    <t>£5.13</t>
-  </si>
-  <si>
-    <t>£6.50 delivery 25 October - 16 November. Details</t>
-  </si>
-  <si>
     <t>The Midnight Library: Matt Haig</t>
   </si>
   <si>
@@ -356,21 +350,9 @@
     <t>The Paper Palace: The No.1 New York Times Bestseller and Reese Witherspoon Bookclub Pick</t>
   </si>
   <si>
-    <t>£7.34</t>
-  </si>
-  <si>
-    <t>£23.83 delivery 16 October - 3 November</t>
-  </si>
-  <si>
     <t>Wilder Girls</t>
   </si>
   <si>
-    <t>£17.12</t>
-  </si>
-  <si>
-    <t>£3.07 delivery 25 October - 16 November. Details</t>
-  </si>
-  <si>
     <t>Carrie Soto Is Back: From the author of The Seven Husbands of Evelyn Hugo (California dream (crossover) serie, 4)</t>
   </si>
   <si>
@@ -410,7 +392,7 @@
     <t>The Seven Husbands of Evelyn Hugo</t>
   </si>
   <si>
-    <t>$13.90 delivery November 3 - 27. Details</t>
+    <t>$13.90 delivery November 3 - 28. Details</t>
   </si>
   <si>
     <t>The Madness of Crowds: A Novel (Chief Inspector Gamache Novel, 17)</t>
@@ -420,8 +402,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -468,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -479,7 +460,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1102,30 +1082,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98DDC17-C3C4-4342-AE6F-9F2989894367}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3CF3CC-0BF5-42B6-8C66-13E54DF5EB88}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.44140625" customWidth="1"/>
+    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
         <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" s="5">
         <v>14.24</v>
@@ -1142,18 +1127,18 @@
         <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
         <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B4" s="5">
         <v>9.9499999999999993</v>
@@ -1170,13 +1155,13 @@
         <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
         <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1198,13 +1183,13 @@
         <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
         <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1226,13 +1211,13 @@
         <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
         <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1254,18 +1239,18 @@
         <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
         <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B12" s="5">
         <v>10.87</v>
@@ -1282,18 +1267,18 @@
         <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C13" t="s">
         <v>82</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B14" s="5">
         <v>11.46</v>
@@ -1310,18 +1295,18 @@
         <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C15" t="s">
         <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B16" s="5">
         <v>18.8</v>
@@ -1349,7 +1334,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
@@ -1357,7 +1342,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
@@ -1365,10 +1350,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C20" s="5">
-        <v>26.37</v>
+        <v>25.84</v>
       </c>
       <c r="D20" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1376,26 +1361,26 @@
         <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
         <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="6">
+        <v>117</v>
+      </c>
+      <c r="B22" s="5">
         <v>15.35</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>21.23</v>
       </c>
     </row>
@@ -1405,12 +1390,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE568AA-7BF7-416F-AC0F-07E1EED96BC1}">
-  <dimension ref="A1:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B777945C-C84E-4D95-B42E-A9424C581F21}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="57.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1533,12 +1521,6 @@
       <c r="B10" t="s">
         <v>82</v>
       </c>
-      <c r="C10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1549,69 +1531,63 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" t="s">
-        <v>105</v>
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1619,84 +1595,54 @@
         <v>81</v>
       </c>
       <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
         <v>82</v>
-      </c>
-      <c r="C18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>112</v>
-      </c>
-      <c r="B24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>